<commit_message>
added original_price and discounted_price on scrapper_tokopedia.py
</commit_message>
<xml_diff>
--- a/Lazada_Moringa_10-03-2025.xlsx
+++ b/Lazada_Moringa_10-03-2025.xlsx
@@ -516,24 +516,24 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jamu herbal kapsul tradisional De Moringa Sari Daun kelor</t>
+          <t>Dar Bumi Paket Bulking Alami Moringa Daun Kelor Bubuk Premium Dan Madu Murni 350 Gram Varian Raw Honey</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rp35.000</t>
+          <t>Rp64.900</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kab. Bandung</t>
+          <t>Kota Jakarta Barat</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>80 Terjual</t>
+          <t>445 Terjual</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/jamu-herbal-kapsul-tradisional-de-moringa-sari-daun-kelor-i8265214431.html</t>
+          <t>https://www.lazada.co.id/products/dar-bumi-paket-bulking-alami-moringa-daun-kelor-bubuk-premium-dan-madu-murni-350-gram-varian-raw-honey-i8249122400.html</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -549,12 +549,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bubuk Daun Kelor Dari Bumi - Moringa Asli Serbuk Kelor Powder Herbal Original</t>
+          <t>Daun Kelor Moringa Bubuk Organik 450 Gr Premium Pure Organik Dari Bumi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rp25.700</t>
+          <t>Rp47.500</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>148 Terjual</t>
+          <t>3.5K Terjual</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -574,7 +574,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-dari-bumi-moringa-asli-serbuk-kelor-powder-herbal-original-i8335998377.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-moringa-bubuk-organik-450-gr-premium-pure-organik-dari-bumi-i7549106805.html</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -582,28 +582,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DAUN KELOR BUBUK DARI BUMI (GRATIS BUMI) DAUN KELOR 50gr,150gr,250gr,450gr,/Daun Kelor Obat Herbal Asam Urat Rematik Diabetes Kanker Rematik/Daun Kelor Moringa Organik Murni Alami/Best Seller Disemua Market</t>
+          <t>Daun Kelor Bubuk Safiya 350 Gram Moringa Powder Original Safiya</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rp36.400</t>
+          <t>Rp12.500</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Kota Jakarta Selatan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+          <t>Kota Jakarta Barat</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2.7K Terjual</t>
+        </is>
+      </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/daun-kelor-bubuk-dari-bumi-gratis-bumi-daun-kelor-50gr150gr250gr450grdaun-kelor-obat-herbal-asam-urat-rematik-diabetes-kanker-rematikdaun-kelor-moringa-organik-murni-alamibest-seller-disemua-market-i8378902865.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-bubuk-safiya-350-gram-moringa-powder-original-safiya-i1669978478.html</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -611,28 +615,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>bubuk daun kelor murni 100% asli tanpa campuran / Moringa powder kemasan 1kg</t>
+          <t>Daun Kelor Moringa Bubuk 400 Gr Premium Pure Organic - Padangb ulan</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rp55.000</t>
+          <t>Rp18.999</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Kota Surabaya</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>Kota Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>261 Terjual</t>
+        </is>
+      </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-murni-100-asli-tanpa-campuran-moringa-powder-kemasan-1kg-i8373222666.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-moringa-bubuk-400-gr-premium-pure-organic-padangb-ulan-i8186644265.html</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -640,24 +648,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MKING - moringa king -jamu herbal multivitamin - cegah virus - bersertifikasi bpom bergaransi 100%</t>
+          <t>Jamu herbal kapsul tradisional De Moringa Sari Daun kelor</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rp250.000</t>
+          <t>Rp35.000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Kota Kediri</t>
+          <t>Kab. Bandung</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>7 Terjual</t>
+          <t>80 Terjual</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -665,7 +673,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/mking-moringa-king-jamu-herbal-multivitamin-cegah-virus-bersertifikasi-bpom-bergaransi-100-i8333302407.html</t>
+          <t>https://www.lazada.co.id/products/jamu-herbal-kapsul-tradisional-de-moringa-sari-daun-kelor-i8265214431.html</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -673,28 +681,32 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>bubuk daun kelor kemasan 1kg, bubuk murni 100% asli tanpa campuran / Moringa powder</t>
+          <t>BELI 2 GRATIS 1 Kapsul Ekstrak Daun Kelor 100 Kapsul Asli 100% Original Moringa Oliefera BPOM Keloreena</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rp50.000</t>
+          <t>Rp69.000</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Kota Surabaya</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Kota Bogor</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>117 Terjual</t>
+        </is>
+      </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-kemasan-1kg-bubuk-murni-100-asli-tanpa-campuran-moringa-powder-i8378660388.html</t>
+          <t>https://www.lazada.co.id/products/beli-2-gratis-1-kapsul-ekstrak-daun-kelor-100-kapsul-asli-100-original-moringa-oliefera-bpom-keloreena-i7951772408.html</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -702,24 +714,24 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bubuk Daun Kelor Moringa 100gr, 250gr, 500gr, 1Kg Organik Superfood Food Grade Multivitamin Asli Original tanpa campuran</t>
+          <t>Daun Kelor Moringa Bubuk Dari Bumi Serbuk Kelor Organik</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rp35.500</t>
+          <t>Rp44.500</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Kab. Bandung</t>
+          <t>Kota Jakarta Barat</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>101 Terjual</t>
+          <t>2.7K Terjual</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -727,7 +739,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-moringa-100gr-250gr-500gr-1kg-organik-superfood-food-grade-multivitamin-asli-original-tanpa-campuran-i8307110932.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-moringa-bubuk-dari-bumi-serbuk-kelor-organik-i1188038662.html</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
@@ -735,24 +747,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Daun Kelor Moringa Bubuk Premium Pure Organic</t>
+          <t>Serbuk Daun Kelor 100 Gram | Powder Moringa Moringa Original Assyifa Ghaniyyu Shop</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rp12.000</t>
+          <t>Rp9.500</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Kota Depok</t>
+          <t>Kota Medan</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>33 Terjual</t>
+          <t>126 Terjual</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -760,7 +772,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/daun-kelor-moringa-bubuk-premium-pure-organic-i8308882670.html</t>
+          <t>https://www.lazada.co.id/products/serbuk-daun-kelor-100-gram-powder-moringa-moringa-original-assyifa-ghaniyyu-shop-i7735282978.html</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -768,28 +780,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>teh DAUN KELOR kering 1KG 1 kg moringa</t>
+          <t>Bubuk Daun Kelor Dari Bumi - Moringa Asli Serbuk Kelor Powder Herbal Original</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rp42.263</t>
+          <t>Rp25.700</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Kab. Blora</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
+          <t>Kota Jakarta Barat</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>148 Terjual</t>
+        </is>
+      </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/teh-daun-kelor-kering-1kg-1-kg-moringa-i8364440643.html</t>
+          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-dari-bumi-moringa-asli-serbuk-kelor-powder-herbal-original-i8335998377.html</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -797,19 +813,19 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jamu Tetes Bio Moringa</t>
+          <t>bubuk daun kelor kemasan 1kg, bubuk murni 100% asli tanpa campuran / Moringa powder</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rp220.000</t>
+          <t>Rp50.000</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Kota Bekasi</t>
+          <t>Kota Surabaya</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -818,7 +834,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/jamu-tetes-bio-moringa-i8381950248.html</t>
+          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-kemasan-1kg-bubuk-murni-100-asli-tanpa-campuran-moringa-powder-i8378660388.html</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -826,19 +842,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DAUN KELOR BUBUK DARI BUMI (GRATIS BUMI) DAUN KELOR 50gr,150gr,250gr,450gr,/Daun Kelor Obat Herbal Asam Urat Rematik Diabetes Kanker Rematik/Daun Kelor Moringa Organik Murni Alami/Best Seller Disemua Market</t>
+          <t>Bubuk Daun Kelor 500gr / Daun Kelor Bubuk / Mnga powder 4CUNK.ID</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rp18.200</t>
+          <t>Rp25.900</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Kota Jakarta Selatan</t>
+          <t>Kab. Cirebon</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -847,7 +863,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/daun-kelor-bubuk-dari-bumi-gratis-bumi-daun-kelor-50gr150gr250gr450grdaun-kelor-obat-herbal-asam-urat-rematik-diabetes-kanker-rematikdaun-kelor-moringa-organik-murni-alamibest-seller-disemua-market-i8378912890.html</t>
+          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-500gr-daun-kelor-bubuk-mnga-powder-4cunkid-i8379026139.html</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -855,19 +871,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>bubuk daun kelor 100gr. murni 100% asli tanpa campuran / Moringa powder</t>
+          <t>DAUN KELOR BUBUK DARI BUMI (GRATIS BUMI) DAUN KELOR 50gr,150gr,250gr,450gr,/Daun Kelor Obat Herbal Asam Urat Rematik Diabetes Kanker Rematik/Daun Kelor Moringa Organik Murni Alami/Best Seller Disemua Market</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Rp6.500</t>
+          <t>Rp36.400</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Kota Surabaya</t>
+          <t>Kota Jakarta Selatan</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -876,7 +892,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-100gr-murni-100-asli-tanpa-campuran-moringa-powder-i8378616304.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-bubuk-dari-bumi-gratis-bumi-daun-kelor-50gr150gr250gr450grdaun-kelor-obat-herbal-asam-urat-rematik-diabetes-kanker-rematikdaun-kelor-moringa-organik-murni-alamibest-seller-disemua-market-i8378902865.html</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -884,19 +900,19 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Minyak Pijat Daun Kelor Plus VCO 100Ml Moringa Leaf Oil Hasil Bumi Indonesia</t>
+          <t>BAYIKU.ID X MORINGA Temo Teh Kelor Asi Booster Teh Pelancar Asi Teh Herbal Anti Oksidan</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Rp9.900</t>
+          <t>Rp25.480</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Kab. Situbondo</t>
+          <t>Kota Malang</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -905,7 +921,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/minyak-pijat-daun-kelor-plus-vco-100ml-moringa-leaf-oil-hasil-bumi-indonesia-i8376916198.html</t>
+          <t>https://www.lazada.co.id/products/bayikuid-x-moringa-temo-teh-kelor-asi-booster-teh-pelancar-asi-teh-herbal-anti-oksidan-i8373564762.html</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
@@ -913,19 +929,19 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Daun Moringa Suplemen - Sumber Vitamin dan Mineral untuk Daya Tahan Tubuh</t>
+          <t>Moringa Tea Osada | Teh daun Kelor</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Rp46.000</t>
+          <t>Rp17.250</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Kab. Tangerang</t>
+          <t>Kab. Sleman</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>
@@ -934,7 +950,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/daun-moringa-suplemen-sumber-vitamin-dan-mineral-untuk-daya-tahan-tubuh-i8376342691.html</t>
+          <t>https://www.lazada.co.id/products/moringa-tea-osada-teh-daun-kelor-i8369658395.html</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
@@ -942,19 +958,19 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>KELOREENA Ekstrak Daun Kelor Asli Moringa Olefeira Standard BPOM dan HALAL MUI Isi 50 &amp; 100 Kapsul</t>
+          <t>bubuk daun kelor 100gr. murni 100% asli tanpa campuran / Moringa powder</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Rp97.500</t>
+          <t>Rp6.500</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Kota Jakarta Pusat</t>
+          <t>Kota Surabaya</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -963,7 +979,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/keloreena-ekstrak-daun-kelor-asli-moringa-olefeira-standard-bpom-dan-halal-mui-isi-50-100-kapsul-i8374108380.html</t>
+          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-100gr-murni-100-asli-tanpa-campuran-moringa-powder-i8378616304.html</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
@@ -971,7 +987,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Aladin Herbal - Keloreena Kapsul Daun Kelor Moringa Oleifera 100% ORIGINAL - MULTIKHASIAT</t>
+          <t>Keloreena Kapsul Ekstrak Daun Kelor Alami Moringa Oleifera Ekstrack HALAL Herbal 50 &amp; 100 Kapsul Garansi BISA COD Aman Tanpa Efek Samping</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -983,16 +999,20 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Kota Jakarta Selatan</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
+          <t>Kota Jakarta Barat</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>3.9K Terjual</t>
+        </is>
+      </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/aladin-herbal-keloreena-kapsul-daun-kelor-moringa-oleifera-100-original-multikhasiat-i8370770225.html</t>
+          <t>https://www.lazada.co.id/products/keloreena-kapsul-ekstrak-daun-kelor-alami-moringa-oleifera-ekstrack-halal-herbal-50-100-kapsul-garansi-bisa-cod-aman-tanpa-efek-samping-i6659588856.html</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1000,28 +1020,32 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ALAMEE Bubuk Minuman Daun Kelor Moringa Powder Serbuk Daun Kelor Herbal Tanpa Gula 250gr</t>
+          <t>M KING / M KING / MORINGA KING JAMU TETES HERBAL ISI 20 ml ORIGINAL</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Rp35.000</t>
+          <t>Rp240.000</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Kota Bekasi</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
+          <t>Kab. Sidoarjo</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>91 Terjual</t>
+        </is>
+      </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/alamee-bubuk-minuman-daun-kelor-moringa-powder-serbuk-daun-kelor-herbal-tanpa-gula-250gr-i8369704810.html</t>
+          <t>https://www.lazada.co.id/products/m-king-m-king-moringa-king-jamu-tetes-herbal-isi-20-ml-original-i7289386512.html</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
@@ -1029,28 +1053,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MOREing Beauty Moringa Gentle Cleanser 100ml - Pembersih Wajah Sabun Muka Wajah</t>
+          <t>Keloreena Kapsul Original (Produk Bergaransi Resmi) - Keloreena 50 Kapsul Dan Keloreena 100 Kapsul Terlaris Asli Ekstrak Daun Kelor Moringa Berkhasiat Atasi Penyakit Degeneratif</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Rp89.000</t>
+          <t>Rp97.500</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Kota Denpasar</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
+          <t>Kota Jakarta Barat</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2.3K Terjual</t>
+        </is>
+      </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/moreing-beauty-moringa-gentle-cleanser-100ml-pembersih-wajah-sabun-muka-wajah-i8365978427.html</t>
+          <t>https://www.lazada.co.id/products/keloreena-kapsul-original-produk-bergaransi-resmi-keloreena-50-kapsul-dan-keloreena-100-kapsul-terlaris-asli-ekstrak-daun-kelor-moringa-berkhasiat-atasi-penyakit-degeneratif-i8209308955.html</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1058,19 +1086,19 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bubuk Serbuk Daun Kelor Moringa isi 50 gram masker minuman</t>
+          <t>Herbilogy Ekstrak Daun Kelor Penambah Nutrisi Tubuh Moringa Extract Powder BPOM - 100 Gr</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Rp4.104</t>
+          <t>Rp99.275</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Kab. Blora</t>
+          <t>Kota Jakarta Utara</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -1079,7 +1107,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-serbuk-daun-kelor-moringa-isi-50-gram-masker-minuman-i8364418369.html</t>
+          <t>https://www.lazada.co.id/products/herbilogy-ekstrak-daun-kelor-penambah-nutrisi-tubuh-moringa-extract-powder-bpom-100-gr-i3965034684.html</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1087,32 +1115,28 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Bubuk Serbuk Daun Kelor isi 250gr teh moringa</t>
+          <t>bubuk daun kelor murni 100% asli tanpa campuran / Moringa powder kemasan 1kg</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Rp11.638</t>
+          <t>Rp55.000</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Kab. Blora</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>6 Terjual</t>
-        </is>
-      </c>
+          <t>Kota Surabaya</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-serbuk-daun-kelor-isi-250gr-teh-moringa-i8364418368.html</t>
+          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-murni-100-asli-tanpa-campuran-moringa-powder-kemasan-1kg-i8373222666.html</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1120,19 +1144,19 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Bubuk Serbuk Daun Kelor isi 100 gram Moringa murni masker minuman</t>
+          <t>Kapsul Daun Kelor Moringa</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Rp6.738</t>
+          <t>Rp17.000</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Kab. Blora</t>
+          <t>Kab. Tangerang</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1141,7 +1165,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-serbuk-daun-kelor-isi-100-gram-moringa-murni-masker-minuman-i8364386580.html</t>
+          <t>https://www.lazada.co.id/products/kapsul-daun-kelor-moringa-i6763204015.html</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
@@ -1149,19 +1173,19 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Biji Kernel Kelor Moringa isi 100 Gram Kupas Kupasan</t>
+          <t>Jamu Tetes Herbal MKING Membantu Menambah Nutrisi dan Meningkatkan Stamina Tubuh - M KING - Moringa King | M-king | M king | Mking Herbal | Vitamin | Obat Herbal | Obat kanker - M King Moringa Jamu tetes Asli Original 100%</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Rp14.088</t>
+          <t>Rp238.900</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Kab. Blora</t>
+          <t>Kab. Kediri</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -1170,7 +1194,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/biji-kernel-kelor-moringa-isi-100-gram-kupas-kupasan-i8364344992.html</t>
+          <t>https://www.lazada.co.id/products/jamu-tetes-herbal-mking-membantu-menambah-nutrisi-dan-meningkatkan-stamina-tubuh-m-king-moringa-king-m-king-m-king-mking-herbal-vitamin-obat-herbal-obat-kanker-m-king-moringa-jamu-tetes-asli-original-100-i8261150583.html</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1178,28 +1202,32 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Moringa Glow - Natural Face Wash</t>
+          <t>BIO MORINGA 20 ML /MORINGA JAMU TETES /Jamu Herbal | Moringa</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Rp43.000</t>
+          <t>Rp193.566</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Kab. Bekasi</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
+          <t>Kab. Sidoarjo</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>68 Terjual</t>
+        </is>
+      </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/moringa-glow-natural-face-wash-i8363902378.html</t>
+          <t>https://www.lazada.co.id/products/bio-moringa-20-ml-moringa-jamu-tetes-jamu-herbal-moringa-i7287598538.html</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -1207,28 +1235,32 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Kapsul daun kelor isi 60 kapsul moringa oleifera</t>
+          <t>Kapsul Ekstrak Daun Kelor BPOM Pro Moringa Ash Shihhah 50 Kp</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rp31.000</t>
+          <t>Rp18.500</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Kota Medan</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
+          <t>Kota Bekasi</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>888 Terjual</t>
+        </is>
+      </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/kapsul-daun-kelor-isi-60-kapsul-moringa-oleifera-i8363584251.html</t>
+          <t>https://www.lazada.co.id/products/kapsul-ekstrak-daun-kelor-bpom-pro-moringa-ash-shihhah-50-kp-i1600334403.html</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1236,28 +1268,32 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Keloreena Asli Original 1 Botol Isi 50 Kapsul Ekstrak Daun Kelor Moringa Obat Kolesterol Darah Tinggi Dan Asam Urat Kolesterol Tinggi Hipertensi Nyeri Sendi Penurun Kolesterol Jahat Syaraf Kejepit Sakit Pinggang</t>
+          <t>Kapsul Daun Kelor / Moringa isi 100. Asli. Alami</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Rp93.350</t>
+          <t>Rp12.000</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Kota Jakarta Selatan</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
+          <t>Kab. Bogor</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>44 Terjual</t>
+        </is>
+      </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/keloreena-asli-original-1-botol-isi-50-kapsul-ekstrak-daun-kelor-moringa-obat-kolesterol-darah-tinggi-dan-asam-urat-kolesterol-tinggi-hipertensi-nyeri-sendi-penurun-kolesterol-jahat-syaraf-kejepit-sakit-pinggang-i8343460525.html</t>
+          <t>https://www.lazada.co.id/products/kapsul-daun-kelor-moringa-isi-100-asli-alami-i7132454298.html</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1265,28 +1301,32 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BOOSTER TEA (Moringa &amp; Ashitaba) kemas teabag</t>
+          <t>Moringa King | M-king | M king | Mking Herbal | Vitamin | Obat Herbal | Obat kanker</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Rp50.000</t>
+          <t>Rp222.277</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Kab. Malang</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
+          <t>Kab. Sidoarjo</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>390 Terjual</t>
+        </is>
+      </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/booster-tea-moringa-ashitaba-kemas-teabag-i8342300543.html</t>
+          <t>https://www.lazada.co.id/products/moringa-king-m-king-m-king-mking-herbal-vitamin-obat-herbal-obat-kanker-i7084614917.html</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1294,28 +1334,32 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Herbana Relief Sari Daun Kelor 400mg Moringa Oleifera 30 Kapsul - Memelihara Kesehatan Tubuh</t>
+          <t>Serbuk Bubuk Daun Kelor murni Powder Moringa 1 Kg</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Rp77.120</t>
+          <t>Rp12.900</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Kab. Bandung</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
+          <t>Kota Tangerang Selatan</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>29 Terjual</t>
+        </is>
+      </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/herbana-relief-sari-daun-kelor-400mg-moringa-oleifera-30-kapsul-memelihara-kesehatan-tubuh-i8339736069.html</t>
+          <t>https://www.lazada.co.id/products/serbuk-bubuk-daun-kelor-murni-powder-moringa-1-kg-i8280830122.html</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -1323,28 +1367,32 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PRO MORINGA Ekstrak Daun Kelor Ash-Shihah untuk menambah zat gizi - EXP : 2027</t>
+          <t>Bubuk Daun Kelor Moringa 100gr, 250gr, 500gr, 1Kg Organik Superfood Food Grade Multivitamin Asli Original tanpa campuran</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Rp17.200</t>
+          <t>Rp35.500</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Kab. Bogor</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
+          <t>Kab. Bandung</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>101 Terjual</t>
+        </is>
+      </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/pro-moringa-ekstrak-daun-kelor-ash-shihah-untuk-menambah-zat-gizi-exp-2027-i8334476469.html</t>
+          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-moringa-100gr-250gr-500gr-1kg-organik-superfood-food-grade-multivitamin-asli-original-tanpa-campuran-i8307110932.html</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -1352,28 +1400,32 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NATUR HAIR SHAMPOO SERIES | Aloevera Argan Oil Ginseng Moringa Tea Tree Oil</t>
+          <t>Serbuk Daun Kelor 350 Gram Safiya Asli Bubuk Moringa Powder Herbal Original</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Rp16.625</t>
+          <t>Rp23.700</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Kota Surabaya</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
+          <t>Kota Jakarta Barat</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>603 Terjual</t>
+        </is>
+      </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/natur-hair-shampoo-series-aloevera-argan-oil-ginseng-moringa-tea-tree-oil-i8333930003.html</t>
+          <t>https://www.lazada.co.id/products/serbuk-daun-kelor-350-gram-safiya-asli-bubuk-moringa-powder-herbal-original-i1187978420.html</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
@@ -1381,28 +1433,32 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BIO MORINGA - obat herbal bersertifikat bpom -manfaat daun kelor-memenuhi asupan nutrisi tubuh</t>
+          <t>Daun Kelor Moringa Bubuk Premium Pure Organik 50 Gr</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Rp220.000</t>
+          <t>Rp12.000</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Kota Kediri</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
+          <t>Kota Tangerang Selatan</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>8 Terjual</t>
+        </is>
+      </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bio-moringa-obat-herbal-bersertifikat-bpom-manfaat-daun-kelor-memenuhi-asupan-nutrisi-tubuh-i8333392752.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-moringa-bubuk-premium-pure-organik-50-gr-i8333854487.html</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1410,28 +1466,32 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>OBAT ANEMIA DEWAS Kapsul Moringa Atasi Anemia Kurang Darah Untuk Anak Anak Dan Dewasa Original BPOM</t>
+          <t>Natur Shampoo Natural Extract Ginseng Aloe Vera Moringa Argan Menyuburkan Menguatkan Rambut Anti Ketombe Lepek 140ml 270ml</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Rp49.999</t>
+          <t>Rp29.498</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Kota Malang</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
+          <t>Kota Tangerang</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>93 Terjual</t>
+        </is>
+      </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/obat-anemia-dewas-kapsul-moringa-atasi-anemia-kurang-darah-untuk-anak-anak-dan-dewasa-original-bpom-i8324614714.html</t>
+          <t>https://www.lazada.co.id/products/natur-shampoo-natural-extract-ginseng-aloe-vera-moringa-argan-menyuburkan-menguatkan-rambut-anti-ketombe-lepek-140ml-270ml-i8307612596.html</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -1439,28 +1499,32 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Kapsul Daun Kelor Murni Moringa 60 Kapsul Ekstrak Daun Kelor Membantu Menjaga Kesehatan Tubuh</t>
+          <t>Daun Kelor Moringa Bubuk Premium Pure Organic</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Rp53.053</t>
+          <t>Rp12.000</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Kab. Malang</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr"/>
+          <t>Kota Depok</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>33 Terjual</t>
+        </is>
+      </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/kapsul-daun-kelor-murni-moringa-60-kapsul-ekstrak-daun-kelor-membantu-menjaga-kesehatan-tubuh-i8324518972.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-moringa-bubuk-premium-pure-organic-i8308882670.html</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -1468,19 +1532,19 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Safiya Daun Kelor 50 Gr Moringa Bubuk 100% Murni Premium</t>
+          <t>Teh Daun Kelor Moringa - Teh Celup Daun Kelor Asli - Obat Herbal Teh Daun Kelor Moringa</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Rp9.500</t>
+          <t>Rp26.000</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Kab. Tangerang</t>
+          <t>Kota Malang</t>
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
@@ -1489,7 +1553,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/safiya-daun-kelor-50-gr-moringa-bubuk-100-murni-premium-i8322366241.html</t>
+          <t>https://www.lazada.co.id/products/teh-daun-kelor-moringa-teh-celup-daun-kelor-asli-obat-herbal-teh-daun-kelor-moringa-i4774272691.html</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -1497,19 +1561,19 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>KAPSUL MORINGA</t>
+          <t>teh DAUN KELOR kering 1KG 1 kg moringa</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Rp30.000</t>
+          <t>Rp42.263</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Kota Bekasi</t>
+          <t>Kab. Blora</t>
         </is>
       </c>
       <c r="F36" t="inlineStr"/>
@@ -1518,7 +1582,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/kapsul-moringa-i8319366071.html</t>
+          <t>https://www.lazada.co.id/products/teh-daun-kelor-kering-1kg-1-kg-moringa-i8364440643.html</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -1526,19 +1590,19 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Kapsul DAUN KELOR SYIFA 60 Kapsul Obat Herbal Daun Kelor Mengatasi Segala Macam Penyakit Kapsul Pro moringa Daun Kelor Syifa</t>
+          <t>Daun kelor kapsul moringa suplemen kesehatan keloreena asi booster dan perawatan kulit organik isi 50 kapsul</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Rp26.500</t>
+          <t>Rp26.000</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Kota Surabaya</t>
+          <t>Kota Semarang</t>
         </is>
       </c>
       <c r="F37" t="inlineStr"/>
@@ -1547,7 +1611,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/kapsul-daun-kelor-syifa-60-kapsul-obat-herbal-daun-kelor-mengatasi-segala-macam-penyakit-kapsul-pro-moringa-daun-kelor-syifa-i8318194925.html</t>
+          <t>https://www.lazada.co.id/products/daun-kelor-kapsul-moringa-suplemen-kesehatan-keloreena-asi-booster-dan-perawatan-kulit-organik-isi-50-kapsul-i7192454754.html</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
@@ -1555,19 +1619,19 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Obat Herbal Daun Kelor Bubuk Original 100% Moringa Powder Grade A</t>
+          <t>BIO MORINGA 20 ML | Daun Kelor | EKSTRAK DAUN KELOR | JAMU TETES KESEHATAN 100% ORIGINAL ORIGINAL</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Rp35.000</t>
+          <t>Rp220.000</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Kota Jakarta Barat</t>
+          <t>Kab. Karawang</t>
         </is>
       </c>
       <c r="F38" t="inlineStr"/>
@@ -1576,7 +1640,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/obat-herbal-daun-kelor-bubuk-original-100-moringa-powder-grade-a-i8315546125.html</t>
+          <t>https://www.lazada.co.id/products/bio-moringa-20-ml-daun-kelor-ekstrak-daun-kelor-jamu-tetes-kesehatan-100-original-original-i7970818234.html</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
@@ -1584,28 +1648,32 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Elora - Moringa Infused Collagen Drink - Paket 18 Hari Cerah &amp; Glowing ( Isi 12 Sachet )</t>
+          <t>Pro Moringa - Kapsul Ekstrak Daun Kelor</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Rp110.500</t>
+          <t>Rp21.348</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Kota Depok</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
+          <t>Kota Medan</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>74 Terjual</t>
+        </is>
+      </c>
       <c r="G39" t="n">
         <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/elora-moringa-infused-collagen-drink-paket-18-hari-cerah-glowing-isi-12-sachet-i8313064983.html</t>
+          <t>https://www.lazada.co.id/products/pro-moringa-kapsul-ekstrak-daun-kelor-i5586144798.html</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -1613,19 +1681,19 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>KAPSUL DAUN KELOR MORINGA 10 PCS HERBAL MURNI ALAMI MANFAAT UNTUK KESEHATAN</t>
+          <t>BUBUK DAUN KELOR 150G DAUN KELOR ORGANIK SERBUK PREMIUM SUPER HALUS BUBUK POWDER MORINGA 100% ORIGINAL PURE ORGANIC NUTRIFARM / BEORGANIK / DARI BUMI / SAFIYA / GALLEO</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Rp2.500</t>
+          <t>Rp46.000</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Kota Jakarta Selatan</t>
+          <t>Kota Bogor</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -1634,7 +1702,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/kapsul-daun-kelor-moringa-10-pcs-herbal-murni-alami-manfaat-untuk-kesehatan-i8303904698.html</t>
+          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-150g-daun-kelor-organik-serbuk-premium-super-halus-bubuk-powder-moringa-100-original-pure-organic-nutrifarm-beorganik-dari-bumi-safiya-galleo-i8302688590.html</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
@@ -1642,28 +1710,32 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>BUBUK DAUN KELOR 150G DAUN KELOR ORGANIK SERBUK PREMIUM SUPER HALUS BUBUK POWDER MORINGA 100% ORIGINAL PURE ORGANIC NUTRIFARM / BEORGANIK / DARI BUMI / SAFIYA / GALLEO</t>
+          <t>Bubuk/serbuk daun kelor moringa oleifera super food murni 1kg</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Rp46.000</t>
+          <t>Rp25.000</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Kota Bogor</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr"/>
+          <t>Kab. Situbondo</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>27 Terjual</t>
+        </is>
+      </c>
       <c r="G41" t="n">
         <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://www.lazada.co.id/products/bubuk-daun-kelor-150g-daun-kelor-organik-serbuk-premium-super-halus-bubuk-powder-moringa-100-original-pure-organic-nutrifarm-beorganik-dari-bumi-safiya-galleo-i8302688590.html</t>
+          <t>https://www.lazada.co.id/products/bubukserbuk-daun-kelor-moringa-oleifera-super-food-murni-1kg-i7582520797.html</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>

</xml_diff>